<commit_message>
added a new row
</commit_message>
<xml_diff>
--- a/JAWS_KNOWLEDGEBASESPREADSHEET__300_EN-1.xlsx
+++ b/JAWS_KNOWLEDGEBASESPREADSHEET__300_EN-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RobertoSantos\Desktop\hitgubrepos\gitnbash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2865C150-B646-4AA3-B8A6-A7B3779DB837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D89EDEF-1143-446F-8BDB-A83D5B9AE436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1845" windowWidth="21600" windowHeight="14355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge Base Entries" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>Comments</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>ERROR Code</t>
   </si>
 </sst>
 </file>
@@ -926,7 +929,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="20.25"/>
@@ -967,7 +970,9 @@
       <c r="H1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="20"/>
+      <c r="I1" s="20" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="2" spans="1:9" ht="408.95" customHeight="1">
       <c r="A2" s="12" t="s">
@@ -1061,7 +1066,7 @@
         <v>29</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>22</v>

</xml_diff>